<commit_message>
Test cases for PA1 - Ethan.
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zee/development/CS151_labs/PA1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eadch\PycharmProjects\cs151-pa1-eadsouza\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0D32F8-6D7A-7B45-9670-B8699C8948C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5526BFB6-88F7-47E4-92D0-580D48EC44DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="67920" windowHeight="28300" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -34,17 +34,124 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>You need to create your own tests</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Decision Point</t>
+  </si>
+  <si>
+    <t>Expected Output</t>
+  </si>
+  <si>
+    <t>"forest"</t>
+  </si>
+  <si>
+    <t>"cave"</t>
+  </si>
+  <si>
+    <t>"river"</t>
+  </si>
+  <si>
+    <t>you venture into the dense forest, surrounded by towering trees and the sounds of wildlife. The journey will not be easy.")</t>
+  </si>
+  <si>
+    <t>you cautiously enter the dark cave, your footsteps echoing off the stone walls. You can barely see ahead, but you press forward.")</t>
+  </si>
+  <si>
+    <t>Initial Stage</t>
+  </si>
+  <si>
+    <t>Door Choice</t>
+  </si>
+  <si>
+    <t>You enter a peaceful clearing. The air is calm, and you feel at ease.</t>
+  </si>
+  <si>
+    <t>You encounter a pack of wild animals. You need to be prepared to handle them.</t>
+  </si>
+  <si>
+    <t>You find a treasure chest in the middle of the room.</t>
+  </si>
+  <si>
+    <t>That's not a valid door. Please select 1, 2, or 3.</t>
+  </si>
+  <si>
+    <t>That's not a valid choice. Please choose 'forest' or 'cave'.</t>
+  </si>
+  <si>
+    <t>Door Choice Test Cases for Cave</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>purple</t>
+  </si>
+  <si>
+    <t>Potion Choice</t>
+  </si>
+  <si>
+    <t>The red potion grants you immense strength!</t>
+  </si>
+  <si>
+    <t>The blue potion grants you invisibility, allowing you to sneak past enemies.</t>
+  </si>
+  <si>
+    <t>That's not a valid potion choice. Please choose 'red', 'blue', or 'green'.</t>
+  </si>
+  <si>
+    <t>The green potion heals you from your injuries.</t>
+  </si>
+  <si>
+    <t>Jump Distance</t>
+  </si>
+  <si>
+    <t>"You fall short of the gap and need to find another way around."</t>
+  </si>
+  <si>
+    <t>"You make it across the gap successfully!"</t>
+  </si>
+  <si>
+    <t>"You overshoot the jump and land in a dangerous spot."</t>
+  </si>
+  <si>
+    <t>"Please enter a valid positive distance to jump across."</t>
+  </si>
+  <si>
+    <t>Potion Choice Test Cases</t>
+  </si>
+  <si>
+    <t>Jump Distance Test Cases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Path Choice </t>
+  </si>
+  <si>
+    <t>Path Choice</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -72,10 +179,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -95,9 +214,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -135,7 +254,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -241,7 +360,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -383,7 +502,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -391,26 +510,233 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF6E1F2-B43E-D343-BB9B-DE90F40B65C5}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="72.9140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="10.6640625" style="4"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="37" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
+        <v>3</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
+        <v>4</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C17" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="4">
+        <v>7</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="4">
+        <v>11</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="4">
+        <v>-5</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C23" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+  <mergeCells count="4">
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="D19:D22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>